<commit_message>
Continue refining unit tests
</commit_message>
<xml_diff>
--- a/cliprt/tests/test_workbook.xlsx
+++ b/cliprt/tests/test_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhodges/VisualStudioCodeProjects/cliprt/cliprt/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1E2EEF-E90C-274C-9578-58F1D7245360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54273795-499A-5C4C-969D-B1B636AAE41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="740" windowWidth="31940" windowHeight="18320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="740" windowWidth="31940" windowHeight="18320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Elements" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="188">
   <si>
     <t>Data Element</t>
   </si>
@@ -473,9 +473,6 @@
     <t>Barclay</t>
   </si>
   <si>
-    <t>barclay@gmailnot</t>
-  </si>
-  <si>
     <t>(999) 888-0001</t>
   </si>
   <si>
@@ -582,6 +579,24 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>LGBTQ</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>barclay@gmail.not</t>
   </si>
 </sst>
 </file>
@@ -1067,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1271,7 +1286,7 @@
         <v>28</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>29</v>
@@ -1283,7 +1298,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>32</v>
@@ -1294,7 +1309,7 @@
         <v>100005800</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C2" s="3">
         <v>43882</v>
@@ -1312,7 +1327,7 @@
         <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>86</v>
@@ -1342,7 +1357,7 @@
         <v>38</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>84</v>
@@ -1372,7 +1387,7 @@
         <v>40</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>88</v>
@@ -1402,7 +1417,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I5" s="21" t="s">
         <v>90</v>
@@ -1432,7 +1447,7 @@
         <v>38</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>93</v>
@@ -1462,7 +1477,7 @@
         <v>45</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I7" s="21" t="s">
         <v>125</v>
@@ -1492,7 +1507,7 @@
         <v>47</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I8" s="21" t="s">
         <v>97</v>
@@ -1516,13 +1531,13 @@
         <v>36</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I9" s="21" t="s">
         <v>100</v>
@@ -1552,7 +1567,7 @@
         <v>40</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I10" s="21" t="s">
         <v>104</v>
@@ -1582,7 +1597,7 @@
         <v>50</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I11" s="21" t="s">
         <v>106</v>
@@ -1608,7 +1623,7 @@
         <v>38</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I12" s="21" t="s">
         <v>107</v>
@@ -1638,7 +1653,7 @@
         <v>40</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I13" s="21" t="s">
         <v>109</v>
@@ -1668,7 +1683,7 @@
         <v>52</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I14" s="21" t="s">
         <v>111</v>
@@ -1698,7 +1713,7 @@
         <v>35</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I15" s="21" t="s">
         <v>113</v>
@@ -1728,7 +1743,7 @@
         <v>52</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16" s="21" t="s">
         <v>115</v>
@@ -1752,13 +1767,13 @@
         <v>51</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I17" s="21" t="s">
         <v>117</v>
@@ -1788,7 +1803,7 @@
         <v>45</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>119</v>
@@ -1812,13 +1827,13 @@
         <v>36</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>54</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I19" s="21" t="s">
         <v>121</v>
@@ -1848,7 +1863,7 @@
         <v>55</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>123</v>
@@ -1875,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L5569"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1884,10 +1899,10 @@
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>56</v>
       </c>
@@ -1903,8 +1918,11 @@
       <c r="E1" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>79</v>
       </c>
@@ -1915,13 +1933,16 @@
         <v>100005800</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>61</v>
       </c>
@@ -1932,13 +1953,16 @@
         <v>100000058</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>62</v>
       </c>
@@ -1949,13 +1973,16 @@
         <v>100005310</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>83</v>
       </c>
@@ -1966,13 +1993,16 @@
         <v>100003575</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>131</v>
       </c>
@@ -1983,13 +2013,16 @@
         <v>100001587</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>133</v>
       </c>
@@ -2000,13 +2033,16 @@
         <v>100001586</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F7" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>135</v>
       </c>
@@ -2017,13 +2053,16 @@
         <v>100000536</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>87</v>
       </c>
@@ -2034,13 +2073,13 @@
         <v>100003465</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>91</v>
       </c>
@@ -2051,13 +2090,16 @@
         <v>100005413</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>137</v>
       </c>
@@ -2068,13 +2110,16 @@
         <v>100000467</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>139</v>
       </c>
@@ -2085,13 +2130,16 @@
         <v>100000468</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E12" s="21" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>141</v>
       </c>
@@ -2102,13 +2150,16 @@
         <v>100001293</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>94</v>
       </c>
@@ -2119,13 +2170,16 @@
         <v>100005723</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>126</v>
       </c>
@@ -2136,13 +2190,13 @@
         <v>100004341</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>143</v>
       </c>
@@ -2153,13 +2207,16 @@
         <v>100000414</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>145</v>
       </c>
@@ -2170,13 +2227,16 @@
         <v>100002322</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>98</v>
       </c>
@@ -2187,13 +2247,16 @@
         <v>100006004</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>101</v>
       </c>
@@ -2204,13 +2267,16 @@
         <v>100003248</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>80</v>
       </c>
@@ -2221,90 +2287,93 @@
         <v>100005827</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="11"/>
       <c r="D21" s="14"/>
       <c r="E21" s="20"/>
     </row>
-    <row r="22" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="11"/>
       <c r="D22" s="15"/>
       <c r="E22" s="20"/>
     </row>
-    <row r="23" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="11"/>
       <c r="D23" s="15"/>
       <c r="E23" s="20"/>
     </row>
-    <row r="24" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="11"/>
       <c r="D24" s="15"/>
       <c r="E24" s="20"/>
     </row>
-    <row r="25" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="C25" s="11"/>
       <c r="D25" s="15"/>
       <c r="E25" s="20"/>
     </row>
-    <row r="26" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="11"/>
       <c r="D26" s="15"/>
       <c r="E26" s="20"/>
     </row>
-    <row r="27" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="11"/>
       <c r="D27" s="15"/>
       <c r="E27" s="20"/>
     </row>
-    <row r="28" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="11"/>
       <c r="D28" s="15"/>
       <c r="E28" s="20"/>
     </row>
-    <row r="29" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="11"/>
       <c r="D29" s="15"/>
       <c r="E29" s="20"/>
     </row>
-    <row r="30" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="11"/>
       <c r="D30" s="15"/>
       <c r="E30" s="20"/>
     </row>
-    <row r="31" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="C31" s="11"/>
       <c r="D31" s="15"/>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="11"/>

</xml_diff>

<commit_message>
Separate de_type from dest_de_format
</commit_message>
<xml_diff>
--- a/cliprt/tests/test_workbook.xlsx
+++ b/cliprt/tests/test_workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhodges/VisualStudioCodeProjects/cliprt/cliprt/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D71A6DD-0420-5040-9F95-F816004208FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE497D2-CB05-8B4B-BF7D-662EF65A5B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="31940" windowHeight="18320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -970,9 +970,6 @@
     <t>Dest DE Format</t>
   </si>
   <si>
-    <t>Dest DE</t>
-  </si>
-  <si>
     <t>Content DE Type</t>
   </si>
   <si>
@@ -980,6 +977,9 @@
   </si>
   <si>
     <t>Content DE Name</t>
+  </si>
+  <si>
+    <t>Dest DE Name</t>
   </si>
 </sst>
 </file>
@@ -1444,7 +1444,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1454,16 +1454,16 @@
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>310</v>
@@ -1549,7 +1549,7 @@
         <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>